<commit_message>
permissionto to view report
</commit_message>
<xml_diff>
--- a/media/excel/detail.xlsx
+++ b/media/excel/detail.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,17 +534,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OrderedDict([('id', 40), ('password', 'pbkdf2_sha256$390000$MUIB8FwHiRDV6Phpz2UsCA$utHSfT/1pqI47SdblTUanKF+KhLFtCOwuLd7kwbrKWA='), ('last_login', '2022-12-04T12:10:25.702914+05:45'), ('is_superuser', False), ('first_name', 'private user'), ('last_name', ''), ('is_staff', False), ('is_active', True), ('date_joined', '2022-11-29T11:35:16.469786+05:45'), ('sex', None), ('phone', '9808098'), ('permanent_address', None), ('email', 'manojdas.py@gmail.com'), ('username', 'user'), ('state_name', 'Madhesh Province'), ('district_name', 'Dhanusha'), ('is_verified', True), ('is_applyForVerified', True), ('apply_role_type', 3), ('company_name', 'private company'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('approved_name', None), ('approved_email', 'manojdas.py@gmail.com'), ('approved_signature', None), ('approved_company_name', 'md company'), ('image', '/media/user/profile/my_photo.JPG'), ('signature', '/media/user/documents/signature_ceo.jpeg'), ('member_admin', 'admin'), ('created_at', '2022-11-29T11:35:16.940528+05:45'), ('updated_at', '2022-12-04T12:07:18.398027+05:45'), ('role', 5), ('groups', []), ('user_permissions', [])])</t>
+          <t>OrderedDict([('id', 40), ('password', 'pbkdf2_sha256$390000$MUIB8FwHiRDV6Phpz2UsCA$utHSfT/1pqI47SdblTUanKF+KhLFtCOwuLd7kwbrKWA='), ('last_login', '2022-12-07T14:17:40.845462+05:45'), ('is_superuser', False), ('first_name', 'private user'), ('last_name', ''), ('is_staff', False), ('is_active', True), ('date_joined', '2022-11-29T11:35:16.469786+05:45'), ('sex', None), ('phone', '9808098'), ('permanent_address', None), ('email', 'manojdas.py@gmail.com'), ('username', 'user'), ('state_name', 'Madhesh Province'), ('district_name', 'Dhanusha'), ('is_verified', True), ('is_applyForVerified', True), ('apply_role_type', 3), ('company_name', 'private company'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('approved_name', None), ('approved_email', 'manojdas.py@gmail.com'), ('approved_signature', None), ('approved_company_name', 'md company'), ('image', '/media/user/profile/my_photo.JPG'), ('signature', '/media/user/documents/signature_ceo.jpeg'), ('member_admin', 'admin'), ('created_at', '2022-11-29T11:35:16.940528+05:45'), ('updated_at', '2022-12-04T12:07:18.398027+05:45'), ('role', 5), ('groups', []), ('user_permissions', [])])</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>OrderedDict([('id', 23), ('owner_full_name', 'private user'), ('company_name', 'private company'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('business_name', 'plywood_industry'), ('business_price_category', 'less_than_2_crode'), ('is_reniew', True), ('payment_rupees', 10000), ('voucher_number', 'None'), ('municipality', 'Mithila'), ('ward_number', '2'), ('tole', 'topa'), ('authorized_capital_of_company', 98), ('paid_up_capital_of_company', 98), ('transaction_amount', 9822), ('tax_amount', 987), ('number_of_employees', 98), ('approved_name', 'central'), ('approved_email', 'central@gmail.com'), ('approved_signature', '/media/user/documents/signature_eLOwzGt.jpeg'), ('approved_company_name', None), ('certificate_citizenship', '/media/user/documents/Doc1_srdTaWL.jpg'), ('certificate_company_registration', '/media/user/documents/Doc2_mG3bf1z.jpg'), ('provisional_account_number', '/media/user/documents/Doc3_VPLgpYj.jpg'), ('auditing', None), ('tax_paid_certificate', '/media/user/documents/Doc1_NohrdG2.jpg'), ('industry_registration', None), ('income_certificate', None), ('member_approved_certificate', None), ('self_declaration_not_on_the_black_list', None), ('bank_voucher', '/media/user/documents/qr-new.jpg'), ('industry_certificate_front_side', '/media/user/documents/my_photo.JPG'), ('industry_certificate_back_side', '/media/user/documents/my_photo_hGyyNkP.JPG'), ('application_certificate', '/media/user/documents/pdfdmd_mceV4Kr.pdf'), ('physical_year', '2078'), ('created_at', '2022-11-29T11:40:29.785957+05:45'), ('updated_at', '2022-12-04T13:18:04.467115+05:45'), ('user', 40)])</t>
+          <t>OrderedDict([('id', 23), ('owner_full_name', 'private user'), ('company_name', 'private company'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('business_name', 'plywood_industry'), ('business_price_category', 'old_unregistered_non_payment'), ('is_reniew', False), ('payment_rupees', 20000), ('voucher_number', 'None'), ('municipality', 'Mithila'), ('ward_number', '2'), ('tole', 'topa'), ('authorized_capital_of_company', 98), ('paid_up_capital_of_company', 98), ('transaction_amount', 456), ('tax_amount', 987), ('number_of_employees', 98), ('approved_name', 'central'), ('approved_email', 'central@gmail.com'), ('approved_signature', '/media/user/documents/signature_eLOwzGt.jpeg'), ('approved_company_name', None), ('certificate_citizenship', '/media/user/documents/Doc1_srdTaWL.jpg'), ('certificate_company_registration', '/media/user/documents/Doc2_mG3bf1z.jpg'), ('provisional_account_number', '/media/user/documents/Doc3_VPLgpYj.jpg'), ('auditing', None), ('tax_paid_certificate', '/media/user/documents/Doc1_NohrdG2.jpg'), ('industry_registration', None), ('income_certificate', None), ('member_approved_certificate', None), ('self_declaration_not_on_the_black_list', None), ('bank_voucher', '/media/user/documents/qr-new.jpg'), ('industry_certificate_front_side', '/media/user/documents/my_photo.JPG'), ('industry_certificate_back_side', '/media/user/documents/my_photo_hGyyNkP.JPG'), ('application_certificate', '/media/user/documents/PDF_SIGNING_USING_DIGITAL_SIGNATURE_-_Google_Docs_4.pdf'), ('physical_year', '2078'), ('created_at', '2022-11-29T11:40:29.785957+05:45'), ('updated_at', '2022-12-09T13:53:51.136588+05:45'), ('user', 40)])</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>approved</t>
+          <t>central_ceo</t>
         </is>
       </c>
       <c r="F2" t="b">
@@ -567,7 +567,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2022-12-04T13:18:04.535319+05:45</t>
+          <t>2022-12-09T13:53:44.554927+05:45</t>
         </is>
       </c>
       <c r="M2" t="b">
@@ -591,7 +591,76 @@
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="n">
-        <v>18</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OrderedDict([('id', 43), ('password', 'pbkdf2_sha256$390000$N7ybMyN8rPjN2PAqbTyebZ$6bP1q2HSE9ne7oSQXLmesj8afNFthAjpKLKBz94DVm8='), ('last_login', '2022-12-04T16:09:10.190495+05:45'), ('is_superuser', False), ('first_name', 'मनोज दास'), ('last_name', ''), ('is_staff', False), ('is_active', True), ('date_joined', '2022-12-04T16:09:09.463723+05:45'), ('sex', 'male'), ('phone', '98080'), ('permanent_address', None), ('email', 'a@gmail.com'), ('username', 'a'), ('state_name', 'Province No. 1'), ('district_name', 'Ilam'), ('is_verified', True), ('is_applyForVerified', True), ('apply_role_type', 5), ('company_name', 'asd'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('approved_name', None), ('approved_email', None), ('approved_signature', None), ('approved_company_name', None), ('image', None), ('signature', None), ('member_admin', 'member'), ('created_at', '2022-12-04T16:09:09.750044+05:45'), ('updated_at', '2022-12-04T17:16:38.929999+05:45'), ('role', 5), ('groups', []), ('user_permissions', [])])</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>OrderedDict([('id', 24), ('owner_full_name', 'a'), ('company_name', 'asd'), ('union_type', 'district'), ('union_name', 'central@gmail.com'), ('business_name', 'plywood_industry'), ('business_price_category', 'less_than_2_crode'), ('is_reniew', False), ('payment_rupees', 10000), ('voucher_number', 'None'), ('municipality', 'Mangsebung'), ('ward_number', '8'), ('tole', '3'), ('authorized_capital_of_company', 87), ('paid_up_capital_of_company', 87), ('transaction_amount', 8797), ('tax_amount', 98), ('number_of_employees', 890), ('approved_name', None), ('approved_email', None), ('approved_signature', None), ('approved_company_name', None), ('certificate_citizenship', None), ('certificate_company_registration', None), ('provisional_account_number', None), ('auditing', None), ('tax_paid_certificate', None), ('industry_registration', None), ('income_certificate', None), ('member_approved_certificate', None), ('self_declaration_not_on_the_black_list', None), ('bank_voucher', None), ('industry_certificate_front_side', None), ('industry_certificate_back_side', None), ('application_certificate', '/media/user/documents/71-72.pdf'), ('physical_year', '2079'), ('created_at', '2022-12-04T16:09:53.993304+05:45'), ('updated_at', '2022-12-07T17:44:22.720251+05:45'), ('user', 43)])</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>central_ceo</t>
+        </is>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2022-12-04T16:09:54.158928+05:45</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2022-12-06T17:31:40.564555+05:45</t>
+        </is>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>3234</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>